<commit_message>
7am to 7pm fine tuned and working
</commit_message>
<xml_diff>
--- a/SolarOpt/wwwroot/xls/NOAA_Solar_Calculations_day.xlsx
+++ b/SolarOpt/wwwroot/xls/NOAA_Solar_Calculations_day.xlsx
@@ -1748,11 +1748,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239614024"/>
-        <c:axId val="239610104"/>
+        <c:axId val="239311048"/>
+        <c:axId val="239314184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239614024"/>
+        <c:axId val="239311048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -1780,13 +1780,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239610104"/>
+        <c:crossAx val="239314184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239610104"/>
+        <c:axId val="239314184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -1798,7 +1798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239614024"/>
+        <c:crossAx val="239311048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="45"/>
@@ -2618,11 +2618,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="239613240"/>
-        <c:axId val="239613632"/>
+        <c:axId val="239308304"/>
+        <c:axId val="239306736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239613240"/>
+        <c:axId val="239308304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2632,7 +2632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239613632"/>
+        <c:crossAx val="239306736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2640,7 +2640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239613632"/>
+        <c:axId val="239306736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2651,7 +2651,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239613240"/>
+        <c:crossAx val="239308304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2698,6 +2698,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4196,11 +4197,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239611280"/>
-        <c:axId val="239615592"/>
+        <c:axId val="239310656"/>
+        <c:axId val="239311440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239611280"/>
+        <c:axId val="239310656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4229,13 +4230,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239615592"/>
+        <c:crossAx val="239311440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.25"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239615592"/>
+        <c:axId val="239311440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4246,7 +4247,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239611280"/>
+        <c:crossAx val="239310656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4671,8 +4672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="L71" sqref="A71:XFD71"/>
+    <sheetView tabSelected="1" topLeftCell="L183" workbookViewId="0">
+      <selection activeCell="AG201" sqref="AG201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
interval and update to disclaimer
</commit_message>
<xml_diff>
--- a/SolarOpt/wwwroot/xls/NOAA_Solar_Calculations_day.xlsx
+++ b/SolarOpt/wwwroot/xls/NOAA_Solar_Calculations_day.xlsx
@@ -126,7 +126,7 @@
     <t>Time Zone (+ to E)</t>
   </si>
   <si>
-    <t>4/12/2018</t>
+    <t>4/24/2018</t>
   </si>
 </sst>
 </file>
@@ -4952,7 +4952,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="5">
-        <v>40.010613</v>
+        <v>40.002285700000009</v>
       </c>
       <c r="D3" s="2" t="str">
         <f ref="D3:D66" t="shared" si="1">$B$7</f>
@@ -5080,7 +5080,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="5">
-        <v>-83.0150304</v>
+        <v>-83.0158697</v>
       </c>
       <c r="D4" s="2" t="str">
         <f t="shared" si="1"/>

</xml_diff>